<commit_message>
cambio en el archivo
</commit_message>
<xml_diff>
--- a/contactos.xlsx
+++ b/contactos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\winda\Desktop\python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42CDD404-8E33-42BB-A637-2E78817872ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE129FF5-F254-4EA5-A16A-C78A55669759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,24 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>telefono</t>
   </si>
   <si>
     <t>mensaje</t>
-  </si>
-  <si>
-    <t>33 1672 0062</t>
-  </si>
-  <si>
-    <t>33 1081 6707</t>
-  </si>
-  <si>
-    <t>prueba 1</t>
-  </si>
-  <si>
-    <t>prueba 2</t>
   </si>
 </sst>
 </file>
@@ -372,7 +360,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -389,21 +377,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-    </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="B3" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D6" s="1"/>

</xml_diff>